<commit_message>
update 4800 iir excel
</commit_message>
<xml_diff>
--- a/4800_iir_llpf_calc.xlsx
+++ b/4800_iir_llpf_calc.xlsx
@@ -1,25 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ninocarrillo/github/N9600A-sim/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C38E0C5-8B92-F44F-BEA8-8906435AC942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15000" yWindow="140" windowWidth="13800" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15000" yWindow="135" windowWidth="13800" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="LoopFilter LPF" sheetId="4" r:id="rId1"/>
     <sheet name="Branch LPF" sheetId="3" r:id="rId2"/>
     <sheet name="Gains" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -136,8 +130,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -496,34 +490,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -534,7 +528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -545,7 +539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -557,7 +551,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -572,7 +566,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -587,7 +581,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -599,7 +593,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -608,7 +602,7 @@
         <v>2.0436401552442991</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -617,7 +611,7 @@
         <v>1.9563598447557011</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -629,7 +623,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -641,7 +635,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -653,7 +647,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -661,7 +655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -669,7 +663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -678,7 +672,7 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -690,7 +684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -702,7 +696,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -723,38 +717,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18.75">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>1800</v>
+        <v>1400</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -765,19 +759,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <f>2*PI()*B2</f>
-        <v>11309.733552923255</v>
+        <v>8796.45943005142</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -792,13 +786,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <f>(2*B3)*TAN(B4*B5/2)</f>
-        <v>11929.350596345139</v>
+        <v>9080.6051197147244</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -807,79 +801,79 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8">
         <f>B6*B5</f>
-        <v>0.82842712474619018</v>
+        <v>0.63059757775796699</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9">
         <f>2+(B8)</f>
-        <v>2.8284271247461903</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.6305975777579671</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10">
         <f>2-B8</f>
-        <v>1.1715728752538097</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1.3694024222420329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <f>B10/B9</f>
-        <v>0.41421356237309498</v>
+        <v>0.52056705055174624</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13">
         <f>B8/B9</f>
-        <v>0.29289321881345248</v>
+        <v>0.23971647472412683</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
         <f>B8/B9</f>
-        <v>0.29289321881345248</v>
+        <v>0.23971647472412683</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -887,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -895,7 +889,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -904,37 +898,37 @@
         <v>32768</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="1">
         <f>ROUND(B21*B13*B18,0)</f>
-        <v>9598</v>
+        <v>7855</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="1">
         <f>ROUND(B21*B14*B18,0)</f>
-        <v>9598</v>
+        <v>7855</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="1">
         <f>ROUND(B21*B12,0)</f>
-        <v>13573</v>
+        <v>17058</v>
       </c>
       <c r="D24" t="s">
         <v>20</v>
@@ -946,23 +940,24 @@
     <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -971,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -980,7 +975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -988,7 +983,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>30</v>
       </c>

</xml_diff>